<commit_message>
feat: adding design patterns - factory method - builder - abstract factory - proxy - dependence injection - decorator
</commit_message>
<xml_diff>
--- a/docs/design-patterns.xlsx
+++ b/docs/design-patterns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="123">
   <si>
     <t xml:space="preserve">Design Patterns com Java</t>
   </si>
@@ -150,13 +150,13 @@
     <t xml:space="preserve">BUILDER</t>
   </si>
   <si>
+    <t xml:space="preserve">1.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Facilita a criação de objetos de forma que podemos setar as propriedades de uma forma dinâmica
 O Construtor de Classe se torna dinâmico e encadeia várias chamadas
 Muito usado para casos de testes para que seja possível a criação de casos validos a serem testados.
 O padrão builder é um padrão que permite a criação passo-a-passo de objetos complexos usando uma sequencia de ações. A construção é controlada por um objeto diretor que apenas precisa conter o tipo dos objetos que deve ser criado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4</t>
   </si>
   <si>
     <t xml:space="preserve">Passo 1
@@ -222,6 +222,530 @@
 										.comNumero("02020")
 										.construir();</t>
   </si>
+  <si>
+    <t xml:space="preserve">ABSTRACT FACTORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O Padrão Abstract Factory fornece uma interface para criar famílias de objetos relacionados ou dependentes sem especificar suas classes concretas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sempre que for refatorar um projeto para um design pattern certifique-se primeiro que os testes unitário estão bem implementados par anão quebrar nada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrupa atributos em uma fabrica que será passada para o construtor encapsulando informações de injeção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 1 
+INTERFACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pegamos da classe principal seus atributos e transformamos em interfaces:
+public class Pagamento {
+		private Operadora operadora;
+	private GestorDeRisco gestorDeRisco;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public interface Operadora {
+	void capturar(String cartao, BigDecimal valor) throws CapturaNaoAutorizadaException;
+	public Long confirmar();
+	}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public interface GestorDeRisco {
+	void avaliarRisco(String cartao, BigDecimal valor) throws AlertaDeRiscoException;
+	}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementamos as interfaces e sobreescrevemos seus metodos
+- E sempre que houver uma nova funcionalidade criamos uma classe e implementamos
+Cielo implements Operadora {...}
+public class ClearSale implements GestorDeRisco {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 3
+INTERFACE FACTORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criamos uma interface para a fabrica, com as assinaturas de criação dos atributos:
+public interface ModuloPagamentoFactory {
+	public Operadora criarOperadora();
+	public GestorDeRisco criarGestorDeRisco();
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 4
+IMPLEMENTATION FACTORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementamos a interface de fabrica e retornamos a classe que precisamos:
+public class PayPalModuloPagamentoFactory implements ModuloPagamentoFactory {…}
+	@Override
+    public Operadora criarOperadora() {
+	    return new Redecard();
+    }
+	@Override
+    public GestorDeRisco criarGestorDeRisco() {
+	    return new ClearSale();
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 5
+CONSTRUCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na classe principal utilizamos a fabrica para construir os atributos:
+public class Pagamento {
+	private Operadora operadora;
+	private GestorDeRisco gestorDeRisco;
+	public Pagamento(ModuloPagamentoFactory moduloPagamentoFactory) {
+	    this.operadora = moduloPagamentoFactory.criarOperadora();
+	    this.gestorDeRisco = moduloPagamentoFactory.criarGestorDeRisco();
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 6
+USE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instaciamos a Factory Implementada e passamos por parâmetro na classe principal de pagamentos e a utilizamos:
+ModuloPagamentoFactory moduloPagamentoFactory = new PagSeguroModuloPagamentoFactory();
+		Pagamento pagamento = new Pagamento(moduloPagamentoFactory);
+pagamento.autorizar("7777.2222", new BigDecimal("5500"));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROXY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O Padrão Proxy fornece um substituto ou representante de outro objeto para controlar o acesso a ele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proxy Remoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controla o acesso ao acesso a objetos que estão em outra JVM
+Em outra JVM pode ser definida como em outra máquina
+Pode controlar questões de rede por exemplo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proxy Virtual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controla o acesso a um recurso cujo a criação seja demorada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proxy de proteção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controla acesso ao recurso com base em permissões
+Controle chamadas à métodos por exemplo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 1
+REPRESENTATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar uma classe proxy que representará a classe original
+Esta classe deve ter as características da classe original ou seja devemos implementar as interfaces que a original possui
+Original:
+public class ContatosXML implements Contatos {
+	private Map&lt;String, String&gt; contatosEmCache = new HashMap&lt;&gt;();
+	public ContatosXML(String... nomesArquivos) {…} //Construtor
+	@Override
+    public String buscarPor(String email) {...}
+}
+Proxy:
+public class ContatosXMLProxy implements Contatos {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 2
+ATTRIBUTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os atributos dessa classe devem ser a classe original e os parâmetros dessa classe, e deve receber em seu construtor o mesmo tipo que será repassado:
+public class ContatosXMLProxy implements Contatos {
+	private ContatosXML contatosXML;
+	private List&lt;String&gt; nomesArquivos;
+	public ContatosXMLProxy(String... nomesArquivos) {
+		this.nomesArquivos = new ArrayList&lt;&gt;(Arrays.asList(nomesArquivos));
+	}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 3
+OVERRIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sobrescrevemos o método original onde recebemos um parâmetro para ser redirecionado.
+	@Override
+	public String buscarPor(String email) {…}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 4
+REDIRECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazer o redirecionamento do parâmetro recebido, tratando ele devidamente instanciando a classeOriginal e chamando o metodoOriginal
+	@Override
+	public String buscarPor(String email) {
+… // trataento de parametro
+			this.contatosXML = new ContatosXML(nomeArquivo); //instancia da classe
+			nome = this.contatosXML.buscarPor(email); //chamada original	
+		return nome;
+	}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instanciar proxy com tipagem da interface
+_x0001__x0001_Contatos contatos = new ContatosXMLProxy("contatos1.xml", "contatos2.xml");
+Chamar o método do proxy que direcioraná ou para o métodoOriginal
+_x0001_    String nome = contatos.buscarPor("jose@email.com");
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBSERVER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O Padrão Observer define uma dependência um-para-muitos entre objetos, então quando o estado de um objeto muda, todos os seus dependentes serão notificados e atualizados automaticamente
+Registra e desregistra uma ação em tempos de execução
+Utiliza Notificador e Observadores de forma que ao ter uma mudança de status no notificador, os observadores apresentam uma ação correspondente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 1
+LISTENER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar uma interface Listener para representar um ouvinte e implementa essa interface:
+public interface Listener { void atualizar(); }
+Public class EmailListener implements Listener { @Override void atualizar(); }
+Registrar quando receber um notificador por constutor:
+	public EmailListener(Notificador notificador) {
+		this.notificador = notificador;  // armazemos para desregistrar caso necessario ao fim de uma ação
+		this.notificador.registrarListener(this);
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 2 
+NOTIFIER INTERFACE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar uma interface para representar um notificador com os metodos que serão utilizados para registrar, desgegistrar, notificar e outros auxiliares.
+public interface Notificador {
+	void registrarListener(Listener listener);
+	void removerListener(Listener listener);
+	void notificarListeners();
+	void novosLancamentosVencidos(List&lt;Lancamento&gt; lancamentosVencidos);
+	List&lt;Lancamento&gt; getLancamentosVencidos();
+	}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 3 
+NOTIFIER IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar um notificador que possuirá uma lista de listeners e os metodos da interface:
+public class NotificadorLancamentosVencidos implements Notificador {
+	private Set&lt;Listener&gt; listeners;
+	private List&lt;Lancamento&gt; lancamentosVencidos;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 4 
+REGISTRATION METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O método de registrar um listener vai adicionar um listener a um SetList, assim como o de reover removerá esse listener.
+	@Override
+    public void registrarListener(Listener listener) {
+	    this.listeners.add(listener);
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 5
+NOTIFIER METOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O método de notificação percorrerá a lista de ouvintes e chamará o método definido na interface de listener, para não haver acoplamento.
+	@Override
+    public void notificarListeners() {
+		for (Listener listener : listeners) {
+			listener.atualizar();
+		}
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 6
+TASK METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A função que agirá como task será executada ao lançar o evento, que nesse caso é um CronJob, ela irá disparar a executção da notificação aos ouvintes:
+	@Override
+    public void novosLancamentosVencidos(List&lt;Lancamento&gt; lancamentosVencidos) {
+		this.lancamentosVencidos = lancamentosVencidos;
+		this.notificarListeners();
+    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 7
+PARAMETERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os parâmentros que serão passados para a função responsável para notificar os listener está representada na interface como getLancamentosVencidos(), que é uma simulação de uma query no banco de dados.
+Ela será chamada pela função definida na interface de listener:
+Deve ser implementada no Listener para ser obtida e repassada:
+Implementação do Notificador:
+	@Override
+    public List&lt;Lancamento&gt; getLancamentosVencidos() {
+	    return this.lancamentosVencidos;
+    }
+Implementação do Listener:
+	@Override
+    public void atualizar() {
+		List&lt;Lancamento&gt; lancamentosVencidos = this.notificador.getLancamentosVencidos();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 8
+SCHEDULE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obtem uma instancia que representa um notificador:
+Notificador notificador = (Notificador) jobDataMap.get("notificador");
+Notificador recebe os dados por parâmetros:
+notificador.novosLancamentosVencidos(lancamentosVencidos);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 9
+EXECUTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faz o Input do notificador
+		Notificador notificador = new NotificadorLancamentosVencidos();
+jobDataMap.put("notificador", notificador);
+Cria os ouvintes, não necessário estar em uma variável.
+		Listener enviadorEmail = new EmailListener(notificador);
+		Listener enviadorSms = new SMSListener(notificador);
+Executa o serviço:
+	scheduler.scheduleJob(job, trigger);
+		scheduler.start();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPENDENCY INJECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Framework de Injeção de dependência do Java EE com CDI
+- Containter que gerencia as dependências de forma automática, assim como os ciclos de vida
+- Possibilita anotações em dependência para que haja uma injeção
+- Torna o código mais limpo evitando instanciar com “new”
+Exemplo de Injeção:
+@Inject private CalculadoraImposto calculadoraImposto;
+Exemplo de  obtenção de Instância:
+PedidoVendaService service = WeldContext.INSTANCE.getBean(PedidoVendaService.class);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificar Serviços e Dependências acopladas e substitui-los por interfaces
+public interface PedidoVendaService { void salvar(PedidoVenda pedidoVenda);}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 2
+CONSTRUCTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definir as interfaces como atributos da classe e passá-los por parâmetro via construtor
+public class PedidoVendaServiceImpl implements PedidoVendaService {
+	private CalculadoraImposto calculadoraImposto;
+	public PedidoVendaService(CalculadoraImposto calculadoraImposto){
+		this.calculadoraImposto = calculadoraImposto;
+	}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1
+Construtor Forma Limpa
+Spring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Service
+@AllArgsConstructor
+public class PedidoVendaServiceImpl implements PedidoVendaService {
+    private final CalculadoraImposto calculadoraImposto;   //Com final e sem Autowired
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 3
+IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar as interfaces e todas as assinaturas dos métodos, de forma que não tenha dependências acopladas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 4
+USE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'- Utilizar a própria interface para obter uma instancia do Serviço Implementado
+CalculadoraImposto c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">alculadora = new CalculadoraImpostoImpl();
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PedidoVendaService service = new PedidoVendaServiceImpl(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">calculadora</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">);
+- Chamar o método conforme a assinatura da interface:
+		service.salvar(pedidoVenda);</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DECORATOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.14</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">O Padrão Decorator anexa responsabilidades adicionais a um objeto dinamicamente. Os decoradores fornecem uma alternativa flexível de subclasse para estender a funcionalidade.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- Anexar responsabilidade adicionais à um objeto, ou seja novos métodos.
+- Segue o princípio “O” do SOLID, que trata-se do princípio de Aberto-Fechado
+- Abertas para extensão e fechadas para modificação
+- Adiciona uma nova responsabilidade sem alterar a classe.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Analisar a classe que implementa uma interface e que precisará de uma nova funcionalidade
+public interface AutorizadorCartaoCredito { void autorizar(Cliente cliente, CartaoCredito cartaoCredito, double valor);}
+public class AutorizadorCielo implements AutorizadorCartaoCredito {…</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">autorizar(..)..</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 2
+DECORATOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar uma Classe que além de implementar a Interface também tenha como atributo a própria Interface para injetar
+public class AnalisadorDeRiscoClearSale implements AutorizadorCartaoCredito {
+	private AutorizadorCartaoCredito autorizador;
+	public AnalisadorDeRiscoClearSale(AutorizadorCartaoCredito autorizador) {
+		this.autorizador = autorizador;
+	}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 3
+REDIRECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementar o método da interface e realizar adicionar nova funcionalidade e redirecionar para o super.metodo da interface injetada.
+	@Override
+	public void autorizar(Cliente cliente, CartaoCredito cartaoCredito, double valor) {
+		if (cliente.getCpf().startsWith("111") || cartaoCredito.getVencimento().isBefore(YearMonth.now())
+				|| valor &gt; 500) {
+			throw new RiscoCreditoException("Possível fraude, negando pagamento!");
+		}
+		autorizador.autorizar(cliente, cartaoCredito, valor);
+	}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construir um objeto baseado na interface e englobar o objeto que era usado anteriormente:
+ANTES:
+AutorizadorCartaoCredito autorizador = new AutorizadorCielo();
+DEPOIS:
+AutorizadorCartaoCredito autorizador = new AnalisadorDeRiscoClearSale(new AutorizadorCielo());</t>
+  </si>
 </sst>
 </file>
 
@@ -230,7 +754,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -265,6 +789,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -328,7 +864,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -369,7 +905,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -556,15 +1096,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="116.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.3"/>
   </cols>
@@ -702,18 +1242,18 @@
       <c r="B15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="104.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="97.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
@@ -725,16 +1265,16 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="99.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="157.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -761,49 +1301,496 @@
       <c r="C21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="C23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="C24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
+    <row r="26" customFormat="false" ht="71.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="C26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
+    <row r="27" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
+    <row r="28" customFormat="false" ht="50.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="C28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
+    <row r="29" customFormat="false" ht="51.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="C29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="72.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="146.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" customFormat="false" ht="139.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="83.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="42.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" customFormat="false" ht="152.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" customFormat="false" ht="134.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="42.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="118.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="71.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8"/>
+      <c r="B44" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="72.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="109" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="123.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" customFormat="false" ht="78.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" customFormat="false" ht="107.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" customFormat="false" ht="101.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" customFormat="false" ht="214.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" customFormat="false" ht="66.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" customFormat="false" ht="134.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="8"/>
+      <c r="B55" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="120.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" customFormat="false" ht="34.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" customFormat="false" ht="112" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" customFormat="false" ht="77.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" customFormat="false" ht="36.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" customFormat="false" ht="84.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8"/>
+      <c r="B62" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="90.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="7"/>
+    </row>
+    <row r="64" customFormat="false" ht="49.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64" s="7"/>
+    </row>
+    <row r="65" customFormat="false" ht="100.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" s="7"/>
+    </row>
+    <row r="66" customFormat="false" ht="137.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="7"/>
+    </row>
+    <row r="67" customFormat="false" ht="80.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="7"/>
+    </row>
+    <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+    </row>
+    <row r="69" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+    </row>
+    <row r="70" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+    </row>
+    <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+    </row>
+    <row r="76" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+    </row>
+    <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+    </row>
+    <row r="79" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+    </row>
+    <row r="80" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+    </row>
+    <row r="81" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B43" r:id="rId1" display="Instanciar proxy com tipagem da interface&#10;_x0001__x0001_Contatos contatos = new ContatosXMLProxy(&quot;contatos1.xml&quot;, &quot;contatos2.xml&quot;);&#10;&#10;Chamar o método do proxy que direcioraná ou para o métodoOriginal&#10;_x0001_    String nome = contatos.buscarPor(&quot;jose@email.com&quot;);&#10;"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
feat: adding design pattern - strategy
</commit_message>
<xml_diff>
--- a/docs/design-patterns.xlsx
+++ b/docs/design-patterns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="131">
   <si>
     <t xml:space="preserve">Design Patterns com Java</t>
   </si>
@@ -410,11 +410,7 @@
 	}</t>
   </si>
   <si>
-    <t xml:space="preserve">Instanciar proxy com tipagem da interface
-_x0001__x0001_Contatos contatos = new ContatosXMLProxy("contatos1.xml", "contatos2.xml");
-Chamar o método do proxy que direcioraná ou para o métodoOriginal
-_x0001_    String nome = contatos.buscarPor("jose@email.com");
-</t>
+    <t xml:space="preserve">Instanciar proxy com tipagem da interface _x0001__x0001_Contatos contatos = new ContatosXMLProxy("contatos1.xml", "contatos2.xml");  Chamar o método do proxy que direcioraná ou para o métodoOriginal _x0001_    String nome = contatos.buscarPor("jose@email.com"); </t>
   </si>
   <si>
     <t xml:space="preserve">OBSERVER</t>
@@ -605,53 +601,11 @@
 USE</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'- Utilizar a própria interface para obter uma instancia do Serviço Implementado
-CalculadoraImposto c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">alculadora = new CalculadoraImpostoImpl();
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PedidoVendaService service = new PedidoVendaServiceImpl(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">calculadora</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">);
+    <t xml:space="preserve">'- Utilizar a própria interface para obter uma instancia do Serviço Implementado
+CalculadoraImposto calculadora = new CalculadoraImpostoImpl();
+PedidoVendaService service = new PedidoVendaServiceImpl(calculadora);
 - Chamar o método conforme a assinatura da interface:
 		service.salvar(pedidoVenda);</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">DECORATOR</t>
@@ -660,57 +614,16 @@
     <t xml:space="preserve">1.14</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">O Padrão Decorator anexa responsabilidades adicionais a um objeto dinamicamente. Os decoradores fornecem uma alternativa flexível de subclasse para estender a funcionalidade.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Anexar responsabilidade adicionais à um objeto, ou seja novos métodos.
+    <t xml:space="preserve">O Padrão Decorator anexa responsabilidades adicionais a um objeto dinamicamente. Os decoradores fornecem uma alternativa flexível de subclasse para estender a funcionalidade.
+- Anexar responsabilidade adicionais à um objeto, ou seja novos métodos.
 - Segue o princípio “O” do SOLID, que trata-se do princípio de Aberto-Fechado
 - Abertas para extensão e fechadas para modificação
 - Adiciona uma nova responsabilidade sem alterar a classe.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Analisar a classe que implementa uma interface e que precisará de uma nova funcionalidade
+  </si>
+  <si>
+    <t xml:space="preserve">Analisar a classe que implementa uma interface e que precisará de uma nova funcionalidade
 public interface AutorizadorCartaoCredito { void autorizar(Cliente cliente, CartaoCredito cartaoCredito, double valor);}
-public class AutorizadorCielo implements AutorizadorCartaoCredito {…</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">autorizar(..)..</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}</t>
-    </r>
+public class AutorizadorCielo implements AutorizadorCartaoCredito {…autorizar(..)..}</t>
   </si>
   <si>
     <t xml:space="preserve">Passo 2
@@ -746,6 +659,63 @@
 DEPOIS:
 AutorizadorCartaoCredito autorizador = new AnalisadorDeRiscoClearSale(new AutorizadorCielo());</t>
   </si>
+  <si>
+    <t xml:space="preserve">STRATEGY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O Padrão Strategy define uma família de algoritmos, encapsula cada um deles e os torna intercambiáveis. O strategy deixa o algoritmo variar independente dos clientes que o utilizam.
+- O strategy veio para resolvel problemas de algoritmos com vários if/else aninhados, facilitando os testes e a manutenção
+- Com strategy cada algoritimo fica separado em uma classe por meio do polimorfismo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Identificar algoritmo que possui várias opções de execução com um padrão e if/else aninhados
+- Criar uma Interface com o nome do método padronizado como assinatura
+public interface Frete { ... calcularPreco(…)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'- Criar classe que implementam a interface e separar logicas dentro do métodos obtido.
+public class Normal implements Frete {
+	@Override calcularPreco(...) {
+		return ... A;
+	}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passo 3
+FACTORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Criar uma fábrica de objetos que com base no Contexto fará uma instanciação de uma Classe implementada
+- Podemos utilizar um Enum ou mesmo uma Abstract Factory:
+public enum TipoFrete {
+	NORMAL {
+		@Override
+		public Frete obterFrete() {
+			return new Normal();
+		}
+	},
+	SEDEX {
+		@Override
+		public Frete obterFrete() {
+			return new Sedex();
+		}
+	};	
+	public abstract Frete obterFrete();	
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Com base em um contexto obtido, definimos através da fábrica qual objeto devemos instanciar
+- Obtemos um contexto
+- Instanciamos um objeto com base na interface
+- Chamamos o método da interface
+- Processamos o algoritmo com base nesse contexto
+int opcaoFrete = entrada.nextInt();
+TipoFrete tipoFrete = TipoFrete.values()[opcaoFrete - 1];
+Frete frete = tipoFrete.obterFrete();
+frete.calcularPreco(distancia);</t>
+  </si>
 </sst>
 </file>
 
@@ -754,7 +724,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -789,18 +759,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -909,7 +867,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1096,10 +1054,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B68" activeCellId="0" sqref="B68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B86" activeCellId="0" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1489,7 +1447,7 @@
       </c>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" customFormat="false" ht="71.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="52.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
         <v>26</v>
       </c>
@@ -1715,82 +1673,98 @@
       <c r="C67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-    </row>
-    <row r="69" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
+      <c r="A68" s="8"/>
+      <c r="B68" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="C69" s="7"/>
     </row>
-    <row r="70" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
+    <row r="70" customFormat="false" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="C70" s="7"/>
     </row>
-    <row r="71" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
+    <row r="71" customFormat="false" ht="66.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C71" s="7"/>
     </row>
-    <row r="72" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
+    <row r="72" customFormat="false" ht="209.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="C72" s="7"/>
     </row>
-    <row r="73" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
+    <row r="73" customFormat="false" ht="125.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="C73" s="7"/>
     </row>
-    <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-    </row>
-    <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-    </row>
-    <row r="76" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-    </row>
-    <row r="77" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-    </row>
-    <row r="78" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-    </row>
-    <row r="79" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-    </row>
-    <row r="80" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-    </row>
-    <row r="81" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0"/>
+      <c r="B74" s="0"/>
+      <c r="C74" s="0"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0"/>
+      <c r="B75" s="0"/>
+      <c r="C75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0"/>
+      <c r="B76" s="0"/>
+      <c r="C76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0"/>
+      <c r="B77" s="0"/>
+      <c r="C77" s="0"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0"/>
+      <c r="B78" s="0"/>
+      <c r="C78" s="0"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0"/>
+      <c r="B79" s="0"/>
+      <c r="C79" s="0"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0"/>
+      <c r="B80" s="0"/>
+      <c r="C80" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B43" r:id="rId1" display="Instanciar proxy com tipagem da interface&#10;_x0001__x0001_Contatos contatos = new ContatosXMLProxy(&quot;contatos1.xml&quot;, &quot;contatos2.xml&quot;);&#10;&#10;Chamar o método do proxy que direcioraná ou para o métodoOriginal&#10;_x0001_    String nome = contatos.buscarPor(&quot;jose@email.com&quot;);&#10;"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>